<commit_message>
Finished Version 1 of program
</commit_message>
<xml_diff>
--- a/cas.xlsx
+++ b/cas.xlsx
@@ -8,94 +8,78 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63995fc1031070f4/Documents/GitHub/chemistry_tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{A8861C20-FA1E-42B3-B1F7-17A705D707E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1728618D-7FDD-4935-BF70-9B16046BEC37}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_0E81EB575E20FD6503334717E69DFD56747B0C31" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9B37808-6ED6-4721-A163-C6D08673F270}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{AEBCC922-68B9-42ED-B45A-7BB4A1CBCE52}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
+    <t>gbg</t>
+  </si>
+  <si>
+    <t>gde</t>
+  </si>
+  <si>
     <t>cas num</t>
   </si>
   <si>
+    <t>ytu</t>
+  </si>
+  <si>
+    <t>duk</t>
+  </si>
+  <si>
     <t>64-17-5</t>
   </si>
   <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>l;l</t>
+  </si>
+  <si>
     <t>64-17-6</t>
   </si>
   <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>mkm</t>
+  </si>
+  <si>
     <t>64-17-7</t>
   </si>
   <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>nmn</t>
+  </si>
+  <si>
     <t>7732-18-5</t>
   </si>
   <si>
-    <t>wewe</t>
-  </si>
-  <si>
-    <t>gbg</t>
-  </si>
-  <si>
-    <t>duk</t>
-  </si>
-  <si>
-    <t>l;l</t>
-  </si>
-  <si>
-    <t>mkm</t>
-  </si>
-  <si>
-    <t>nmn</t>
+    <t>u</t>
   </si>
   <si>
     <t>hhhh</t>
   </si>
   <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>njn</t>
+  </si>
+  <si>
     <t>7-732-185</t>
-  </si>
-  <si>
-    <t>njn</t>
-  </si>
-  <si>
-    <t>ytu</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>g</t>
   </si>
   <si>
     <t>m</t>
@@ -105,16 +89,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,10 +135,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,88 +433,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9005EAB4-4FDC-4A3F-8875-3586739E3913}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -549,25 +527,24 @@
         <v>64175</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>